<commit_message>
web scrapping and pyaudibles and audible files
</commit_message>
<xml_diff>
--- a/Automatic Birthday Wisher/Data.xlsx
+++ b/Automatic Birthday Wisher/Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>sl no</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>happy birthday prabhas</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
 </sst>
 </file>
@@ -447,18 +450,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" customWidth="1"/>
+    <col min="6" max="6" width="113.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -472,13 +480,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -491,14 +502,17 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>8310145281</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="F2">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -511,14 +525,17 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>8147490519</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -526,19 +543,22 @@
         <v>12</v>
       </c>
       <c r="C4" s="2">
-        <v>33089</v>
+        <v>33129</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>8147490519</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="F4">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -546,19 +566,22 @@
         <v>15</v>
       </c>
       <c r="C5" s="2">
-        <v>34185</v>
+        <v>33128</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <v>8310145281</v>
+      </c>
+      <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="F5">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -566,19 +589,22 @@
         <v>18</v>
       </c>
       <c r="C6" s="2">
-        <v>34185</v>
+        <v>34224</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <v>8310145281</v>
+      </c>
+      <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="F6">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -591,14 +617,17 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7">
+        <v>8310145281</v>
+      </c>
+      <c r="F7" t="s">
         <v>20</v>
       </c>
-      <c r="F7">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -611,14 +640,17 @@
       <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8">
+        <v>8310145281</v>
+      </c>
+      <c r="F8" t="s">
         <v>22</v>
       </c>
-      <c r="F8">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -631,10 +663,13 @@
       <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
+        <v>8310145281</v>
+      </c>
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>2019</v>
       </c>
     </row>

</xml_diff>